<commit_message>
bulk upload done and checks done accordingly
</commit_message>
<xml_diff>
--- a/mfi/bulkWork/bulkdeposit.xlsx
+++ b/mfi/bulkWork/bulkdeposit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\sekani\mfi\bulkWork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB7B7586-A130-4A30-978C-5D51ABEC1CBF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8AD026D-1D67-4519-8566-14425C9F75DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1560" yWindow="1560" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,15 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="2">
   <si>
     <t>wuse</t>
   </si>
   <si>
     <t>James Inalegwu Adakole</t>
-  </si>
-  <si>
-    <t>23-11-2020</t>
   </si>
 </sst>
 </file>
@@ -69,8 +66,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -354,7 +352,7 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -363,7 +361,7 @@
     <col min="2" max="2" width="20" customWidth="1"/>
     <col min="3" max="3" width="22.7109375" customWidth="1"/>
     <col min="4" max="4" width="16.85546875" customWidth="1"/>
-    <col min="5" max="5" width="15" customWidth="1"/>
+    <col min="5" max="5" width="15" style="1" customWidth="1"/>
     <col min="7" max="7" width="21.140625" customWidth="1"/>
     <col min="8" max="8" width="11.42578125" customWidth="1"/>
   </cols>
@@ -381,17 +379,17 @@
       <c r="D1">
         <v>8161883854</v>
       </c>
-      <c r="E1" t="s">
-        <v>2</v>
+      <c r="E1" s="1">
+        <v>44159</v>
       </c>
       <c r="F1">
-        <v>5000</v>
+        <v>1000000</v>
       </c>
       <c r="G1">
         <v>3497</v>
       </c>
       <c r="H1">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -407,8 +405,8 @@
       <c r="D2">
         <v>8161883854</v>
       </c>
-      <c r="E2" t="s">
-        <v>2</v>
+      <c r="E2" s="1">
+        <v>44159</v>
       </c>
       <c r="F2">
         <v>5000</v>
@@ -417,7 +415,7 @@
         <v>3498</v>
       </c>
       <c r="H2">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -433,17 +431,17 @@
       <c r="D3">
         <v>8161883854</v>
       </c>
-      <c r="E3" t="s">
-        <v>2</v>
+      <c r="E3" s="1">
+        <v>44159</v>
       </c>
       <c r="F3">
-        <v>5000</v>
+        <v>1000000</v>
       </c>
       <c r="G3">
         <v>3499</v>
       </c>
       <c r="H3">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -459,17 +457,17 @@
       <c r="D4">
         <v>8161883854</v>
       </c>
-      <c r="E4" t="s">
-        <v>2</v>
+      <c r="E4" s="1">
+        <v>44159</v>
       </c>
       <c r="F4">
-        <v>5000</v>
+        <v>1000000</v>
       </c>
       <c r="G4">
         <v>3410</v>
       </c>
       <c r="H4">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>